<commit_message>
columns added in manager query
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -148,10 +148,10 @@
     <t xml:space="preserve">CLUSTER</t>
   </si>
   <si>
-    <t xml:space="preserve">BV Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BVTYPE</t>
+    <t xml:space="preserve">Site Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SITETYPE</t>
   </si>
   <si>
     <t xml:space="preserve">WorkType</t>
@@ -606,8 +606,8 @@
   </sheetPr>
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
default types sheet updated
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="134">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t xml:space="preserve">PGROUPIDENTIFIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SITEGROUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEOPLEGROUP</t>
   </si>
   <si>
     <t xml:space="preserve">Unit</t>
@@ -604,10 +616,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -715,7 +727,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>8</v>
@@ -732,7 +744,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>8</v>
@@ -862,13 +874,13 @@
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>8</v>
@@ -879,13 +891,13 @@
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>8</v>
@@ -896,13 +908,13 @@
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>8</v>
@@ -919,7 +931,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>8</v>
@@ -936,7 +948,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>8</v>
@@ -953,7 +965,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>8</v>
@@ -970,7 +982,7 @@
         <v>45</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>8</v>
@@ -987,7 +999,7 @@
         <v>47</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>8</v>
@@ -1004,7 +1016,7 @@
         <v>49</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>8</v>
@@ -1021,7 +1033,7 @@
         <v>51</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>8</v>
@@ -1038,7 +1050,7 @@
         <v>53</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>8</v>
@@ -1055,7 +1067,7 @@
         <v>55</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>8</v>
@@ -1072,7 +1084,7 @@
         <v>57</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>8</v>
@@ -1089,7 +1101,7 @@
         <v>59</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>8</v>
@@ -1106,7 +1118,7 @@
         <v>61</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>8</v>
@@ -1123,7 +1135,7 @@
         <v>63</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>8</v>
@@ -1140,7 +1152,7 @@
         <v>65</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>8</v>
@@ -1157,7 +1169,7 @@
         <v>67</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>8</v>
@@ -1174,7 +1186,7 @@
         <v>69</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>8</v>
@@ -1191,7 +1203,7 @@
         <v>71</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>8</v>
@@ -1208,7 +1220,7 @@
         <v>73</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>8</v>
@@ -1225,7 +1237,7 @@
         <v>75</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>8</v>
@@ -1242,7 +1254,7 @@
         <v>77</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>8</v>
@@ -1259,7 +1271,7 @@
         <v>79</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>8</v>
@@ -1276,7 +1288,7 @@
         <v>81</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>8</v>
@@ -1293,7 +1305,7 @@
         <v>83</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>8</v>
@@ -1310,7 +1322,7 @@
         <v>85</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>8</v>
@@ -1327,7 +1339,7 @@
         <v>87</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>8</v>
@@ -1344,7 +1356,7 @@
         <v>89</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>8</v>
@@ -1361,7 +1373,7 @@
         <v>91</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>8</v>
@@ -1378,7 +1390,7 @@
         <v>93</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>8</v>
@@ -1395,7 +1407,7 @@
         <v>95</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>8</v>
@@ -1412,7 +1424,7 @@
         <v>97</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>8</v>
@@ -1429,7 +1441,7 @@
         <v>99</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>8</v>
@@ -1446,7 +1458,7 @@
         <v>101</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>8</v>
@@ -1463,7 +1475,7 @@
         <v>103</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>8</v>
@@ -1480,7 +1492,7 @@
         <v>105</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>8</v>
@@ -1497,7 +1509,7 @@
         <v>107</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>8</v>
@@ -1514,7 +1526,7 @@
         <v>109</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>8</v>
@@ -1531,7 +1543,7 @@
         <v>111</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>8</v>
@@ -1548,7 +1560,7 @@
         <v>113</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>8</v>
@@ -1565,7 +1577,7 @@
         <v>115</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>8</v>
@@ -1582,7 +1594,7 @@
         <v>117</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>8</v>
@@ -1599,7 +1611,7 @@
         <v>119</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>8</v>
@@ -1616,7 +1628,7 @@
         <v>121</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>8</v>
@@ -1633,7 +1645,7 @@
         <v>123</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>8</v>
@@ -1650,7 +1662,7 @@
         <v>125</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>8</v>
@@ -1667,7 +1679,7 @@
         <v>127</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>8</v>
@@ -1684,19 +1696,53 @@
         <v>129</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F63" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B64" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B65" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
written test cases attendance view
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="178">
   <si>
     <t>Code*</t>
   </si>
@@ -555,7 +555,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +573,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -615,7 +621,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -926,7 +932,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -2435,40 +2441,6 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="16.5">
-      <c r="A89" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="16.5">
-      <c r="A90" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
breaktime addition in sitetour bulk import cdrf toke issue fixed only show questionsets which have questions in it added list of peoples you can view on click group link
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="181">
   <si>
     <t>Code*</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Asset Type</t>
+  </si>
+  <si>
+    <t>HVAC_SYSTEM</t>
+  </si>
+  <si>
+    <t>HVAC System</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>ASSETCATEGORY</t>
@@ -555,7 +564,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,12 +582,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -610,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -621,7 +624,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -932,17 +938,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="35.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="35.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1255,25 +1261,25 @@
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="C19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>7</v>
@@ -1287,10 +1293,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>7</v>
@@ -1304,10 +1310,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>7</v>
@@ -1321,13 +1327,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>7</v>
@@ -1338,13 +1344,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>7</v>
@@ -1355,13 +1361,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>7</v>
@@ -1372,13 +1378,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>7</v>
@@ -1389,13 +1395,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>7</v>
@@ -1406,13 +1412,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>7</v>
@@ -1423,13 +1429,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>7</v>
@@ -1440,10 +1446,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>28</v>
@@ -1457,10 +1463,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>28</v>
@@ -1474,13 +1480,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>7</v>
@@ -1491,13 +1497,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>7</v>
@@ -1508,13 +1514,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>7</v>
@@ -1525,13 +1531,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>7</v>
@@ -1542,13 +1548,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>7</v>
@@ -1559,13 +1565,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>7</v>
@@ -1576,13 +1582,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>7</v>
@@ -1593,13 +1599,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>7</v>
@@ -1610,13 +1616,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>7</v>
@@ -1627,13 +1633,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>7</v>
@@ -1644,13 +1650,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>7</v>
@@ -1661,13 +1667,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>7</v>
@@ -1678,13 +1684,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
@@ -1695,13 +1701,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>7</v>
@@ -1712,13 +1718,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>7</v>
@@ -1729,13 +1735,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>7</v>
@@ -1746,13 +1752,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>7</v>
@@ -1763,13 +1769,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>7</v>
@@ -1780,13 +1786,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>7</v>
@@ -1797,13 +1803,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>7</v>
@@ -1814,13 +1820,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>7</v>
@@ -1831,13 +1837,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>7</v>
@@ -1848,13 +1854,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>7</v>
@@ -1865,13 +1871,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>7</v>
@@ -1882,13 +1888,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>7</v>
@@ -1899,13 +1905,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>7</v>
@@ -1916,13 +1922,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>7</v>
@@ -1933,13 +1939,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>7</v>
@@ -1950,13 +1956,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>7</v>
@@ -1967,13 +1973,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>7</v>
@@ -1984,13 +1990,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>7</v>
@@ -2001,13 +2007,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>7</v>
@@ -2018,13 +2024,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>7</v>
@@ -2035,13 +2041,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>7</v>
@@ -2052,13 +2058,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>7</v>
@@ -2069,13 +2075,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>7</v>
@@ -2086,13 +2092,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>7</v>
@@ -2103,13 +2109,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>7</v>
@@ -2120,13 +2126,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>7</v>
@@ -2137,13 +2143,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>7</v>
@@ -2154,13 +2160,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>7</v>
@@ -2171,13 +2177,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>7</v>
@@ -2188,13 +2194,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>7</v>
@@ -2205,13 +2211,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>7</v>
@@ -2222,13 +2228,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>7</v>
@@ -2239,13 +2245,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="1" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>7</v>
@@ -2256,13 +2262,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="1" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>7</v>
@@ -2273,13 +2279,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>7</v>
@@ -2290,13 +2296,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>7</v>
@@ -2305,15 +2311,15 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>7</v>
@@ -2322,12 +2328,12 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>7</v>
@@ -2339,50 +2345,50 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
+      <c r="A84" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="16.5">
-      <c r="A84" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C84" s="3" t="s">
+      <c r="D84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
+      <c r="A85" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="16.5">
-      <c r="A85" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="D85" s="3" t="s">
         <v>7</v>
       </c>
@@ -2390,33 +2396,33 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C86" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
+      <c r="A87" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="16.5">
-      <c r="A87" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="D87" s="3" t="s">
         <v>7</v>
       </c>
@@ -2424,20 +2430,37 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B88" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="B88" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
+      <c r="A89" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E88" s="4" t="s">
+      <c r="D89" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
client url mapping for mobile new colored icons added
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="191">
   <si>
     <t>Code*</t>
   </si>
@@ -106,166 +106,169 @@
     <t>Electrical</t>
   </si>
   <si>
+    <t>TC_SITECRISIS</t>
+  </si>
+  <si>
+    <t>Site Crisis</t>
+  </si>
+  <si>
+    <t>NOTIFYCATEGORY</t>
+  </si>
+  <si>
+    <t>Notify Category</t>
+  </si>
+  <si>
+    <t>DEVICERUNNINGSTATUS</t>
+  </si>
+  <si>
+    <t>Device Running Status</t>
+  </si>
+  <si>
+    <t>DEVICEEVENTTYPE</t>
+  </si>
+  <si>
+    <t>Device Event Type</t>
+  </si>
+  <si>
+    <t>LOCATIONTYPE</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>DEVICETYPE</t>
+  </si>
+  <si>
+    <t>Device Type</t>
+  </si>
+  <si>
+    <t>ASSETTYPE</t>
+  </si>
+  <si>
+    <t>Asset Type</t>
+  </si>
+  <si>
+    <t>HVAC_SYSTEM</t>
+  </si>
+  <si>
+    <t>HVAC System</t>
+  </si>
+  <si>
+    <t>ASSETCATEGORY</t>
+  </si>
+  <si>
+    <t>Asset Category</t>
+  </si>
+  <si>
+    <t>ASSETSUBCATEGORY</t>
+  </si>
+  <si>
+    <t>Asset SubCategory</t>
+  </si>
+  <si>
+    <t>ASSETBRAND</t>
+  </si>
+  <si>
+    <t>Asset Brand</t>
+  </si>
+  <si>
+    <t>BVIDENTIFIER</t>
+  </si>
+  <si>
+    <t>BV Identifier</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>SITE</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>BRANCH</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>ZONE</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>CLUSTER</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>SITETYPE</t>
+  </si>
+  <si>
+    <t>Site Type</t>
+  </si>
+  <si>
+    <t>AUTOCLOSENOTIFY</t>
+  </si>
+  <si>
+    <t>Autoclose &amp; Notify</t>
+  </si>
+  <si>
+    <t>AUTOCLOSED</t>
+  </si>
+  <si>
+    <t>Autoclosed</t>
+  </si>
+  <si>
+    <t>RAISETICKETNOTIFY</t>
+  </si>
+  <si>
+    <t>Raise Ticket &amp; Notify</t>
+  </si>
+  <si>
+    <t>WAREHOUSE</t>
+  </si>
+  <si>
+    <t>WareHouse</t>
+  </si>
+  <si>
+    <t>OTHERSITE</t>
+  </si>
+  <si>
+    <t>Other Site</t>
+  </si>
+  <si>
+    <t>SERVICES</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>CUSTOMER</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>EVENTTYPE</t>
+  </si>
+  <si>
+    <t>Event Type</t>
+  </si>
+  <si>
     <t>SITECRISIS</t>
-  </si>
-  <si>
-    <t>Site Crisis</t>
-  </si>
-  <si>
-    <t>NOTIFYCATEGORY</t>
-  </si>
-  <si>
-    <t>Notify Category</t>
-  </si>
-  <si>
-    <t>DEVICERUNNINGSTATUS</t>
-  </si>
-  <si>
-    <t>Device Running Status</t>
-  </si>
-  <si>
-    <t>DEVICEEVENTTYPE</t>
-  </si>
-  <si>
-    <t>Device Event Type</t>
-  </si>
-  <si>
-    <t>LOCATIONTYPE</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>DEVICETYPE</t>
-  </si>
-  <si>
-    <t>Device Type</t>
-  </si>
-  <si>
-    <t>ASSETTYPE</t>
-  </si>
-  <si>
-    <t>Asset Type</t>
-  </si>
-  <si>
-    <t>HVAC_SYSTEM</t>
-  </si>
-  <si>
-    <t>HVAC System</t>
-  </si>
-  <si>
-    <t>ASSETCATEGORY</t>
-  </si>
-  <si>
-    <t>Asset Category</t>
-  </si>
-  <si>
-    <t>ASSETSUBCATEGORY</t>
-  </si>
-  <si>
-    <t>Asset SubCategory</t>
-  </si>
-  <si>
-    <t>ASSETBRAND</t>
-  </si>
-  <si>
-    <t>Asset Brand</t>
-  </si>
-  <si>
-    <t>BVIDENTIFIER</t>
-  </si>
-  <si>
-    <t>BV Identifier</t>
-  </si>
-  <si>
-    <t>CLIENT</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>SITE</t>
-  </si>
-  <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>BRANCH</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>ZONE</t>
-  </si>
-  <si>
-    <t>Zone</t>
-  </si>
-  <si>
-    <t>CLUSTER</t>
-  </si>
-  <si>
-    <t>Cluster</t>
-  </si>
-  <si>
-    <t>SITETYPE</t>
-  </si>
-  <si>
-    <t>Site Type</t>
-  </si>
-  <si>
-    <t>AUTOCLOSENOTIFY</t>
-  </si>
-  <si>
-    <t>Autoclose &amp; Notify</t>
-  </si>
-  <si>
-    <t>AUTOCLOSED</t>
-  </si>
-  <si>
-    <t>Autoclosed</t>
-  </si>
-  <si>
-    <t>RAISETICKETNOTIFY</t>
-  </si>
-  <si>
-    <t>Raise Ticket &amp; Notify</t>
-  </si>
-  <si>
-    <t>WAREHOUSE</t>
-  </si>
-  <si>
-    <t>WareHouse</t>
-  </si>
-  <si>
-    <t>OTHERSITE</t>
-  </si>
-  <si>
-    <t>Other Site</t>
-  </si>
-  <si>
-    <t>SERVICES</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>CUSTOMER</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>PROJECT</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>EVENTTYPE</t>
-  </si>
-  <si>
-    <t>Event Type</t>
   </si>
   <si>
     <t>FIRE</t>
@@ -646,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -655,9 +658,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
@@ -977,11 +977,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="35.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="35.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1666,7 +1666,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="1" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>31</v>
@@ -1683,13 +1683,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>7</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>7</v>
@@ -1717,13 +1717,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
@@ -1734,13 +1734,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
       <c r="A45" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>7</v>
@@ -1751,13 +1751,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
       <c r="A46" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>7</v>
@@ -1768,13 +1768,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
       <c r="A47" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>7</v>
@@ -1785,13 +1785,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
       <c r="A48" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>7</v>
@@ -1802,10 +1802,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>82</v>
@@ -1819,10 +1819,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>82</v>
@@ -1836,10 +1836,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>82</v>
@@ -1853,10 +1853,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>82</v>
@@ -1870,10 +1870,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>82</v>
@@ -1887,10 +1887,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>82</v>
@@ -1904,10 +1904,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>82</v>
@@ -1921,10 +1921,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>82</v>
@@ -1938,10 +1938,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>82</v>
@@ -1955,10 +1955,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>82</v>
@@ -1972,10 +1972,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>82</v>
@@ -1989,10 +1989,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>82</v>
@@ -2006,10 +2006,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>82</v>
@@ -2023,10 +2023,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>82</v>
@@ -2040,10 +2040,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>82</v>
@@ -2057,10 +2057,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>82</v>
@@ -2074,10 +2074,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>82</v>
@@ -2091,10 +2091,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>82</v>
@@ -2108,10 +2108,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>7</v>
@@ -2125,13 +2125,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>7</v>
@@ -2142,13 +2142,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>7</v>
@@ -2159,13 +2159,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>7</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>7</v>
@@ -2193,13 +2193,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>7</v>
@@ -2210,13 +2210,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>7</v>
@@ -2227,13 +2227,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>7</v>
@@ -2244,13 +2244,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>7</v>
@@ -2261,13 +2261,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>7</v>
@@ -2278,13 +2278,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>7</v>
@@ -2295,10 +2295,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>7</v>
@@ -2312,13 +2312,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>7</v>
@@ -2329,13 +2329,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>7</v>
@@ -2346,10 +2346,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>52</v>
@@ -2363,10 +2363,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>52</v>
@@ -2380,13 +2380,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>7</v>
@@ -2397,10 +2397,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>7</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>7</v>
@@ -2431,13 +2431,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>7</v>
@@ -2448,13 +2448,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>7</v>
@@ -2465,13 +2465,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>7</v>
@@ -2482,10 +2482,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>7</v>
@@ -2499,10 +2499,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>7</v>
@@ -2522,7 +2522,7 @@
         <v>29</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>7</v>
@@ -2533,10 +2533,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>12</v>
@@ -2550,13 +2550,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>7</v>
@@ -2567,10 +2567,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>5</v>
@@ -2584,35 +2584,35 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B95" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C95" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E95" s="5" t="s">
+      <c r="B95" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
       <c r="A96" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B96" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="B96" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D96" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E96" s="5" t="s">
+      <c r="D96" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
issues fixed asset comparision added
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -594,7 +594,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,12 +612,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -649,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -658,9 +652,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -977,11 +968,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="35.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="35.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1664,14 +1655,14 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -1688,7 +1679,7 @@
       <c r="B42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -1705,7 +1696,7 @@
       <c r="B43" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -1722,7 +1713,7 @@
       <c r="B44" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D44" s="3" t="s">
@@ -1732,14 +1723,14 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D45" s="3" t="s">
@@ -1749,14 +1740,14 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -1766,14 +1757,14 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -1783,14 +1774,14 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D48" s="3" t="s">

</xml_diff>

<commit_message>
working on new requirements
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="193">
   <si>
     <t>Code*</t>
   </si>
@@ -31,13 +31,19 @@
     <t>Bu*</t>
   </si>
   <si>
+    <t>NOTES_TYPE</t>
+  </si>
+  <si>
+    <t>Notes Type</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
     <t>PEOPLETYPE</t>
   </si>
   <si>
     <t>People Type</t>
-  </si>
-  <si>
-    <t>NONE</t>
   </si>
   <si>
     <t>WORKTYPE</t>
@@ -643,12 +649,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -962,17 +971,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="35.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="35.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -992,7 +1001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1002,10 +1011,10 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1013,16 +1022,16 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1030,16 +1039,16 @@
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1047,16 +1056,16 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1064,16 +1073,16 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1081,16 +1090,16 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1098,16 +1107,16 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1115,16 +1124,16 @@
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1132,16 +1141,16 @@
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1149,16 +1158,16 @@
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1166,16 +1175,16 @@
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1183,16 +1192,16 @@
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1200,16 +1209,16 @@
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1217,16 +1226,16 @@
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1234,16 +1243,16 @@
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1251,16 +1260,16 @@
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="C17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1268,16 +1277,16 @@
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="C18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1285,16 +1294,16 @@
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1302,16 +1311,16 @@
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="C20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1319,16 +1328,16 @@
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1336,16 +1345,16 @@
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="C22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1353,16 +1362,16 @@
       <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="C23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1370,16 +1379,16 @@
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="C24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1387,16 +1396,16 @@
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="C25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1404,16 +1413,16 @@
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="C26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1421,16 +1430,16 @@
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1438,16 +1447,16 @@
       <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="C28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1455,16 +1464,16 @@
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="C29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1472,16 +1481,16 @@
       <c r="A30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="C30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1489,16 +1498,16 @@
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="C31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1506,16 +1515,16 @@
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1523,16 +1532,16 @@
       <c r="A33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="C33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1540,16 +1549,16 @@
       <c r="A34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="C34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1557,16 +1566,16 @@
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="C35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1574,16 +1583,16 @@
       <c r="A36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="C36" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1591,16 +1600,16 @@
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="C37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1608,16 +1617,16 @@
       <c r="A38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="C38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1625,16 +1634,16 @@
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="C39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1642,16 +1651,16 @@
       <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="C40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1659,33 +1668,33 @@
       <c r="A41" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="B41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="D42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1693,16 +1702,16 @@
       <c r="A43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="C43" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1710,16 +1719,16 @@
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="C44" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1727,16 +1736,16 @@
       <c r="A45" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="C45" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1744,16 +1753,16 @@
       <c r="A46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="C46" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1761,16 +1770,16 @@
       <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="C47" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1778,16 +1787,16 @@
       <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="C48" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1795,16 +1804,16 @@
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="C49" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1812,16 +1821,16 @@
       <c r="A50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="C50" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1829,16 +1838,16 @@
       <c r="A51" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="C51" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1846,16 +1855,16 @@
       <c r="A52" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="C52" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1863,16 +1872,16 @@
       <c r="A53" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="C53" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1880,16 +1889,16 @@
       <c r="A54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="C54" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1897,16 +1906,16 @@
       <c r="A55" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="C55" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1914,16 +1923,16 @@
       <c r="A56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="C56" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1931,16 +1940,16 @@
       <c r="A57" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="C57" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1948,16 +1957,16 @@
       <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="C58" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1965,16 +1974,16 @@
       <c r="A59" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="C59" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1982,16 +1991,16 @@
       <c r="A60" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="C60" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1999,16 +2008,16 @@
       <c r="A61" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="C61" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2016,16 +2025,16 @@
       <c r="A62" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="3" t="s">
+      <c r="C62" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2033,16 +2042,16 @@
       <c r="A63" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="C63" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2050,16 +2059,16 @@
       <c r="A64" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="C64" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2067,16 +2076,16 @@
       <c r="A65" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65" s="3" t="s">
+      <c r="C65" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2084,16 +2093,16 @@
       <c r="A66" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E66" s="3" t="s">
+      <c r="C66" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2101,16 +2110,16 @@
       <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" s="3" t="s">
+      <c r="C67" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2118,16 +2127,16 @@
       <c r="A68" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="C68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2135,16 +2144,16 @@
       <c r="A69" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E69" s="3" t="s">
+      <c r="C69" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2152,16 +2161,16 @@
       <c r="A70" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="C70" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2169,16 +2178,16 @@
       <c r="A71" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E71" s="3" t="s">
+      <c r="C71" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2186,16 +2195,16 @@
       <c r="A72" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" s="3" t="s">
+      <c r="C72" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2203,16 +2212,16 @@
       <c r="A73" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="3" t="s">
+      <c r="C73" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2220,16 +2229,16 @@
       <c r="A74" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="C74" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2237,16 +2246,16 @@
       <c r="A75" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75" s="3" t="s">
+      <c r="C75" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2254,16 +2263,16 @@
       <c r="A76" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" s="3" t="s">
+      <c r="C76" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2271,16 +2280,16 @@
       <c r="A77" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E77" s="3" t="s">
+      <c r="C77" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2288,16 +2297,16 @@
       <c r="A78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E78" s="3" t="s">
+      <c r="C78" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2305,16 +2314,16 @@
       <c r="A79" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79" s="3" t="s">
+      <c r="C79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2322,16 +2331,16 @@
       <c r="A80" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E80" s="3" t="s">
+      <c r="C80" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2339,16 +2348,16 @@
       <c r="A81" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" s="3" t="s">
+      <c r="C81" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2356,16 +2365,16 @@
       <c r="A82" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82" s="3" t="s">
+      <c r="C82" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2373,16 +2382,16 @@
       <c r="A83" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E83" s="3" t="s">
+      <c r="C83" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2390,50 +2399,50 @@
       <c r="A84" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84" s="3" t="s">
+      <c r="C84" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E85" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="3" t="s">
+      <c r="D86" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2441,16 +2450,16 @@
       <c r="A87" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E87" s="3" t="s">
+      <c r="C87" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2458,16 +2467,16 @@
       <c r="A88" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E88" s="3" t="s">
+      <c r="C88" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2475,16 +2484,16 @@
       <c r="A89" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89" s="3" t="s">
+      <c r="C89" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2492,50 +2501,50 @@
       <c r="A90" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E90" s="3" t="s">
+      <c r="C90" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E91" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B92" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="3" t="s">
+      <c r="D92" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2543,16 +2552,16 @@
       <c r="A93" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E93" s="3" t="s">
+      <c r="C93" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2560,16 +2569,16 @@
       <c r="A94" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E94" s="3" t="s">
+      <c r="C94" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2577,33 +2586,50 @@
       <c r="A95" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
+      <c r="C95" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E96" s="3" t="s">
+      <c r="C96" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+      <c r="A97" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on schedule report
</commit_message>
<xml_diff>
--- a/docs/default_types.xlsx
+++ b/docs/default_types.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="195">
   <si>
     <t>Code*</t>
   </si>
@@ -419,6 +419,12 @@
   </si>
   <si>
     <t>Diversion</t>
+  </si>
+  <si>
+    <t>SITEVISIT</t>
+  </si>
+  <si>
+    <t>Site Visit</t>
   </si>
   <si>
     <t>GEOFENCE</t>
@@ -600,7 +606,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +618,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -649,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -657,10 +669,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -971,20 +986,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="35.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="35.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1052,7 +1067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1069,7 +1084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1086,7 +1101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1103,7 +1118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1120,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1137,7 +1152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1154,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1171,7 +1186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1188,7 +1203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1205,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1239,7 +1254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1256,7 +1271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1273,7 +1288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1290,7 +1305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1307,7 +1322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -1324,7 +1339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1341,7 +1356,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
@@ -1358,7 +1373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1375,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -1392,7 +1407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1409,7 +1424,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1426,7 +1441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -1443,7 +1458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
@@ -1460,7 +1475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1477,7 +1492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1" t="s">
         <v>62</v>
       </c>
@@ -1494,7 +1509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
@@ -1511,7 +1526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
@@ -1528,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1" t="s">
         <v>68</v>
       </c>
@@ -1545,7 +1560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
         <v>70</v>
       </c>
@@ -2106,14 +2121,14 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="16.5">
       <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D67" s="4" t="s">
@@ -2131,7 +2146,7 @@
         <v>138</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>7</v>
@@ -2148,7 +2163,7 @@
         <v>140</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>137</v>
+        <v>7</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>7</v>
@@ -2165,7 +2180,7 @@
         <v>142</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>7</v>
@@ -2182,7 +2197,7 @@
         <v>144</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>7</v>
@@ -2199,7 +2214,7 @@
         <v>146</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>7</v>
@@ -2216,7 +2231,7 @@
         <v>148</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>7</v>
@@ -2233,7 +2248,7 @@
         <v>150</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>7</v>
@@ -2250,7 +2265,7 @@
         <v>152</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>7</v>
@@ -2267,7 +2282,7 @@
         <v>154</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>7</v>
@@ -2284,7 +2299,7 @@
         <v>156</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>7</v>
@@ -2301,7 +2316,7 @@
         <v>158</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>7</v>
@@ -2318,7 +2333,7 @@
         <v>160</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>7</v>
@@ -2335,7 +2350,7 @@
         <v>162</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>159</v>
+        <v>7</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>7</v>
@@ -2352,7 +2367,7 @@
         <v>164</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>7</v>
@@ -2369,7 +2384,7 @@
         <v>166</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>7</v>
@@ -2403,7 +2418,7 @@
         <v>170</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>137</v>
+        <v>54</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>7</v>
@@ -2420,7 +2435,7 @@
         <v>172</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>7</v>
@@ -2431,13 +2446,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="1" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>171</v>
+        <v>7</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>7</v>
@@ -2448,13 +2463,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>7</v>
@@ -2471,7 +2486,7 @@
         <v>176</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>7</v>
@@ -2488,7 +2503,7 @@
         <v>178</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>7</v>
@@ -2505,7 +2520,7 @@
         <v>180</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>7</v>
@@ -2533,13 +2548,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="1" t="s">
-        <v>30</v>
+        <v>183</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>31</v>
+        <v>184</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>181</v>
+        <v>7</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>7</v>
@@ -2550,13 +2565,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>7</v>
@@ -2573,7 +2588,7 @@
         <v>186</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>7</v>
@@ -2590,7 +2605,7 @@
         <v>188</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>8</v>
+        <v>139</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>7</v>
@@ -2607,7 +2622,7 @@
         <v>190</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>7</v>
@@ -2616,7 +2631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="1" t="s">
         <v>191</v>
       </c>
@@ -2624,12 +2639,29 @@
         <v>192</v>
       </c>
       <c r="C97" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
+      <c r="A98" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C98" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D97" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E97" s="4" t="s">
+      <c r="D98" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>